<commit_message>
Update after 2018-10-14 meeting (off-session)
</commit_message>
<xml_diff>
--- a/Files/Concurrent Engineering/Trade-off.xlsx
+++ b/Files/Concurrent Engineering/Trade-off.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tolosat\Ingénierie Système\Concurrent Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\TOLOSAT\tolosat_systems_engineering\Files\Concurrent Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{54AE4E3C-7C36-4D89-B89A-772CA1789D43}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{435D47E0-7B23-4B4A-8F8D-0EEA8F8AF50D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Trade-off</t>
   </si>
@@ -64,12 +63,15 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Conclusion: OCDT will not be used because of its complexity and unstability. While CDP4 offers more stability and a much more complete software than OCDT, IDM is simple of use, quite complete and should be quite to set up. Also, for Concurrent Engineering, IDM offers simple and efficient solutions for budgets calculus. CDP4 may be used if serious problems are encountered with the installation of IDM.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,18 +232,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -292,6 +285,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,11 +619,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2D230B-F59B-4A0D-9637-32D67994E6AC}">
-  <dimension ref="D4:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,165 +631,308 @@
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E4" s="2" t="s">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D6" s="1"/>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>2</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>4</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <v>3</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>3</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>2.5</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="9">
         <v>2</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D8" s="1"/>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>4</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <v>4</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="9">
         <v>3</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D9" s="1"/>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="7">
         <v>3</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>2</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="9">
         <v>3</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D10" s="1"/>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="7">
         <v>4</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <v>5</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="9">
         <v>3</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="14">
         <v>3</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="10">
         <v>4</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="15">
         <v>2</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="12">
         <f>SUM(F6:F11)</f>
         <v>19</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="17">
         <f>($F6*G6+$F7*G7+$F8*G8+$F9*G9+$F10*G10+$F11*G11)/$F12</f>
         <v>3.6578947368421053</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="18">
         <f t="shared" ref="H12:I12" si="0">($F6*H6+$F7*H7+$F8*H8+$F9*H9+$F10*H10+$F11*H11)/$F12</f>
         <v>2.6842105263157894</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="16">
         <f t="shared" si="0"/>
         <v>3.2105263157894739</v>
       </c>
     </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B14:M23"/>
     <mergeCell ref="E4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>